<commit_message>
Ažurirane tablice i uneseni podaci za sve tablice
</commit_message>
<xml_diff>
--- a/BP2-Projekt_Upravljanje_vinarijom_ERP_sustav.xlsx
+++ b/BP2-Projekt_Upravljanje_vinarijom_ERP_sustav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\FIPU\Druga godina\Baze podataka 2\Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34BE895-B7D7-46BD-A5FC-786E61AB581B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C41336-F740-4DE3-A332-608014D28974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{87F66409-35C4-456F-BC62-BC56FFE0C1BA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="105">
   <si>
     <t>ERP SUSTAV VINARIJE</t>
   </si>
@@ -186,18 +186,12 @@
     <t>datum_pocetka</t>
   </si>
   <si>
-    <t>datum_zavrsetka</t>
-  </si>
-  <si>
     <t>kolicina</t>
   </si>
   <si>
     <t>lokacija</t>
   </si>
   <si>
-    <t>rok_trajanja</t>
-  </si>
-  <si>
     <t>Transport</t>
   </si>
   <si>
@@ -240,9 +234,6 @@
     <t>Proizvod</t>
   </si>
   <si>
-    <t>datum_punjenja</t>
-  </si>
-  <si>
     <t>id_kupac</t>
   </si>
   <si>
@@ -297,9 +288,6 @@
     <t>Racun</t>
   </si>
   <si>
-    <t>id_transport</t>
-  </si>
-  <si>
     <t>Zahtjev_za_nabavu</t>
   </si>
   <si>
@@ -355,6 +343,27 @@
   </si>
   <si>
     <t>status_transporta</t>
+  </si>
+  <si>
+    <t>volumen</t>
+  </si>
+  <si>
+    <t>id_berba</t>
+  </si>
+  <si>
+    <t>Berba</t>
+  </si>
+  <si>
+    <t>Punjenje</t>
+  </si>
+  <si>
+    <t>oznaka_serije</t>
+  </si>
+  <si>
+    <t>pocetak_punjenja</t>
+  </si>
+  <si>
+    <t>zavrsetak_punjenja</t>
   </si>
 </sst>
 </file>
@@ -863,7 +872,7 @@
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="5:8" x14ac:dyDescent="0.25">
@@ -927,10 +936,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B2FB6F-F6FF-4612-A9A6-E7441E4E2505}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,7 +960,7 @@
     <col min="17" max="17" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
@@ -961,23 +970,25 @@
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J1" s="4"/>
+      <c r="I1" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="K1" s="4" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="L1" s="4"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M1" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -996,48 +1007,57 @@
       <c r="K2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I3" t="s">
         <v>43</v>
       </c>
       <c r="K3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="M3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
         <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="K4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="M4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1045,93 +1065,90 @@
         <v>40</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I5" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="K5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I6" t="s">
-        <v>78</v>
-      </c>
-      <c r="K6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="M6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7" t="s">
-        <v>48</v>
-      </c>
-      <c r="K7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="M7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
         <v>42</v>
       </c>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="3"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="G13" s="3" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1150,245 +1167,254 @@
       <c r="K14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" t="s">
+        <v>66</v>
+      </c>
+      <c r="K15" t="s">
+        <v>51</v>
+      </c>
+      <c r="M15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" t="s">
         <v>64</v>
       </c>
-      <c r="E15" t="s">
-        <v>69</v>
-      </c>
-      <c r="G15" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" t="s">
-        <v>43</v>
-      </c>
-      <c r="K15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="I17" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" t="s">
+        <v>45</v>
+      </c>
+      <c r="M17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" t="s">
+        <v>68</v>
+      </c>
+      <c r="M18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>74</v>
       </c>
-      <c r="E16" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" t="s">
-        <v>44</v>
-      </c>
-      <c r="I16" t="s">
-        <v>89</v>
-      </c>
-      <c r="K16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" t="s">
+        <v>94</v>
+      </c>
+      <c r="M19" t="s">
         <v>46</v>
       </c>
-      <c r="G17" t="s">
-        <v>45</v>
-      </c>
-      <c r="I17" t="s">
-        <v>90</v>
-      </c>
-      <c r="K17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" t="s">
-        <v>71</v>
-      </c>
-      <c r="G18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I18" t="s">
-        <v>46</v>
-      </c>
-      <c r="K18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>98</v>
-      </c>
-      <c r="I19" t="s">
-        <v>47</v>
-      </c>
-      <c r="K19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I22" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" t="s">
+        <v>38</v>
+      </c>
+      <c r="K23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" t="s">
+        <v>93</v>
+      </c>
+      <c r="K24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" t="s">
+        <v>83</v>
+      </c>
+      <c r="G25" t="s">
+        <v>70</v>
+      </c>
+      <c r="I25" t="s">
+        <v>77</v>
+      </c>
+      <c r="K25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+      <c r="G26" t="s">
+        <v>62</v>
+      </c>
+      <c r="I26" t="s">
+        <v>48</v>
+      </c>
+      <c r="K26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" t="s">
+        <v>64</v>
+      </c>
+      <c r="G27" t="s">
+        <v>63</v>
+      </c>
+      <c r="I27" t="s">
         <v>49</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" t="s">
-        <v>38</v>
-      </c>
-      <c r="I23" t="s">
-        <v>38</v>
-      </c>
-      <c r="K23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" t="s">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" t="s">
+        <v>95</v>
+      </c>
+      <c r="G28" t="s">
         <v>74</v>
       </c>
-      <c r="E24" t="s">
-        <v>56</v>
-      </c>
-      <c r="G24" t="s">
-        <v>56</v>
-      </c>
-      <c r="I24" t="s">
+      <c r="I28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
         <v>97</v>
-      </c>
-      <c r="K24" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" t="s">
-        <v>87</v>
-      </c>
-      <c r="E25" t="s">
-        <v>73</v>
-      </c>
-      <c r="G25" t="s">
-        <v>73</v>
-      </c>
-      <c r="I25" t="s">
-        <v>80</v>
-      </c>
-      <c r="K25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>90</v>
-      </c>
-      <c r="C26" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" t="s">
-        <v>65</v>
-      </c>
-      <c r="G26" t="s">
-        <v>65</v>
-      </c>
-      <c r="I26" t="s">
-        <v>50</v>
-      </c>
-      <c r="K26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" t="s">
-        <v>66</v>
-      </c>
-      <c r="G27" t="s">
-        <v>66</v>
-      </c>
-      <c r="I27" t="s">
-        <v>51</v>
-      </c>
-      <c r="K27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" t="s">
-        <v>99</v>
-      </c>
-      <c r="E28" t="s">
-        <v>77</v>
-      </c>
-      <c r="G28" t="s">
-        <v>77</v>
-      </c>
-      <c r="I28" t="s">
-        <v>52</v>
-      </c>
-      <c r="K28" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I30" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Materijalizirani pogledi i triggeri
</commit_message>
<xml_diff>
--- a/BP2-Projekt_Upravljanje_vinarijom_ERP_sustav.xlsx
+++ b/BP2-Projekt_Upravljanje_vinarijom_ERP_sustav.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vid\Desktop\BazePodataka2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\FIPU\Druga godina\Baze podataka 2\Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DF793B-D5D4-4EA3-95B5-CE2968BDD836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7036481-CD3F-4CC6-8DD2-865542AD978F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{87F66409-35C4-456F-BC62-BC56FFE0C1BA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="110">
   <si>
     <t>ERP SUSTAV VINARIJE</t>
   </si>
@@ -367,6 +367,18 @@
   </si>
   <si>
     <t>mp_stanje_skladišta_vina</t>
+  </si>
+  <si>
+    <t>jedinicna_cijena</t>
+  </si>
+  <si>
+    <t>Stanje_skladista_vina</t>
+  </si>
+  <si>
+    <t>Stanje_skladista_proizvoda</t>
+  </si>
+  <si>
+    <t>Stanje_skladista_repromaterijala</t>
   </si>
 </sst>
 </file>
@@ -448,13 +460,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalno" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -470,9 +482,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema sustava Office 2013 – 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -510,7 +522,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -616,7 +628,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -774,8 +786,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
@@ -949,10 +961,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B2FB6F-F6FF-4612-A9A6-E7441E4E2505}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,7 +1267,7 @@
         <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="G18" t="s">
         <v>67</v>
@@ -1271,9 +1283,6 @@
       <c r="A19" t="s">
         <v>74</v>
       </c>
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
       <c r="G19" t="s">
         <v>94</v>
       </c>
@@ -1301,7 +1310,7 @@
       <c r="K22" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="M22" s="6" t="s">
+      <c r="M22" s="5" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1433,6 +1442,41 @@
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I30" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Novi materijalizirani pogled (tablica)
</commit_message>
<xml_diff>
--- a/BP2-Projekt_Upravljanje_vinarijom_ERP_sustav.xlsx
+++ b/BP2-Projekt_Upravljanje_vinarijom_ERP_sustav.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\FIPU\Druga godina\Baze podataka 2\Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7036481-CD3F-4CC6-8DD2-865542AD978F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCEDECE-1EF5-4FB2-AB7A-D05EDB7294E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{87F66409-35C4-456F-BC62-BC56FFE0C1BA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="111">
   <si>
     <t>ERP SUSTAV VINARIJE</t>
   </si>
@@ -379,6 +379,9 @@
   </si>
   <si>
     <t>Stanje_skladista_repromaterijala</t>
+  </si>
+  <si>
+    <t>Prodani_proizvodi</t>
   </si>
 </sst>
 </file>
@@ -961,10 +964,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B2FB6F-F6FF-4612-A9A6-E7441E4E2505}">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,8 +1459,11 @@
       <c r="E32" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G32" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>99</v>
       </c>
@@ -1467,8 +1473,11 @@
       <c r="E33" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -1477,6 +1486,14 @@
       </c>
       <c r="E34" t="s">
         <v>45</v>
+      </c>
+      <c r="G34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Izmjena nove tablice i njene procedure
</commit_message>
<xml_diff>
--- a/BP2-Projekt_Upravljanje_vinarijom_ERP_sustav.xlsx
+++ b/BP2-Projekt_Upravljanje_vinarijom_ERP_sustav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\FIPU\Druga godina\Baze podataka 2\Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCEDECE-1EF5-4FB2-AB7A-D05EDB7294E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FC352D-FA24-49E2-9EBF-3961B4E91AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{87F66409-35C4-456F-BC62-BC56FFE0C1BA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="113">
   <si>
     <t>ERP SUSTAV VINARIJE</t>
   </si>
@@ -381,7 +381,13 @@
     <t>Stanje_skladista_repromaterijala</t>
   </si>
   <si>
-    <t>Prodani_proizvodi</t>
+    <t>Kvartalni_pregled_prodaje</t>
+  </si>
+  <si>
+    <t>pocetni_datum</t>
+  </si>
+  <si>
+    <t>zavrsni_datum</t>
   </si>
 </sst>
 </file>
@@ -964,10 +970,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B2FB6F-F6FF-4612-A9A6-E7441E4E2505}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1496,6 +1502,16 @@
         <v>67</v>
       </c>
     </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G37" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Narudžbe i transporti povezani dodatkom atributa id_transport u tablicu zahtjev za narudžbu
</commit_message>
<xml_diff>
--- a/BP2-Projekt_Upravljanje_vinarijom_ERP_sustav.xlsx
+++ b/BP2-Projekt_Upravljanje_vinarijom_ERP_sustav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\FIPU\Druga godina\Baze podataka 2\Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FC352D-FA24-49E2-9EBF-3961B4E91AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CA19EB-80EF-407C-928C-22A4B1F4F1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{87F66409-35C4-456F-BC62-BC56FFE0C1BA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="114">
   <si>
     <t>ERP SUSTAV VINARIJE</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t>zavrsni_datum</t>
+  </si>
+  <si>
+    <t>id_transport</t>
   </si>
 </sst>
 </file>
@@ -970,10 +973,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B2FB6F-F6FF-4612-A9A6-E7441E4E2505}">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,7 +1262,7 @@
         <v>82</v>
       </c>
       <c r="G17" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
       <c r="I17" t="s">
         <v>45</v>
@@ -1279,7 +1282,7 @@
         <v>106</v>
       </c>
       <c r="G18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I18" t="s">
         <v>68</v>
@@ -1293,222 +1296,227 @@
         <v>74</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="M19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3" t="s">
+      <c r="F23" s="3"/>
+      <c r="G23" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="K23" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="M22" s="5" t="s">
+      <c r="M23" s="5" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" t="s">
-        <v>38</v>
-      </c>
-      <c r="I23" t="s">
-        <v>38</v>
-      </c>
-      <c r="K23" t="s">
-        <v>38</v>
-      </c>
-      <c r="M23" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="E24" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="G24" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="I24" t="s">
-        <v>93</v>
+        <v>38</v>
       </c>
       <c r="K24" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="M24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="E25" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="G25" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="I25" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="K25" t="s">
-        <v>66</v>
+        <v>71</v>
+      </c>
+      <c r="M25" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E26" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="G26" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="I26" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="K26" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s">
+        <v>86</v>
+      </c>
+      <c r="E27" t="s">
         <v>45</v>
       </c>
-      <c r="C27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" t="s">
-        <v>64</v>
-      </c>
       <c r="G27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I27" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="K27" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" t="s">
+        <v>63</v>
+      </c>
+      <c r="I28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>46</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>46</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>95</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G29" t="s">
         <v>74</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I29" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I29" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="I30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3" t="s">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3" t="s">
+      <c r="D34" s="3"/>
+      <c r="E34" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G34" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>99</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>51</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E35" t="s">
         <v>83</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>45</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C36" t="s">
         <v>45</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E36" t="s">
         <v>45</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G36" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G35" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G36" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G38" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G39" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Martine transakcije/triggeri i moje izmjene
</commit_message>
<xml_diff>
--- a/BP2-Projekt_Upravljanje_vinarijom_ERP_sustav.xlsx
+++ b/BP2-Projekt_Upravljanje_vinarijom_ERP_sustav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\FIPU\Druga godina\Baze podataka 2\Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CA19EB-80EF-407C-928C-22A4B1F4F1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE53A103-E622-44F7-A7D7-56A367BB11E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{87F66409-35C4-456F-BC62-BC56FFE0C1BA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="113">
   <si>
     <t>ERP SUSTAV VINARIJE</t>
   </si>
@@ -384,13 +384,10 @@
     <t>Kvartalni_pregled_prodaje</t>
   </si>
   <si>
-    <t>pocetni_datum</t>
-  </si>
-  <si>
-    <t>zavrsni_datum</t>
-  </si>
-  <si>
     <t>id_transport</t>
+  </si>
+  <si>
+    <t>kvartal</t>
   </si>
 </sst>
 </file>
@@ -973,10 +970,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24B2FB6F-F6FF-4612-A9A6-E7441E4E2505}">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,7 +1259,7 @@
         <v>82</v>
       </c>
       <c r="G17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I17" t="s">
         <v>45</v>
@@ -1512,11 +1509,6 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G38" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G39" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>